<commit_message>
pareto-front + railroads + params
</commit_message>
<xml_diff>
--- a/resources/excel_config.xlsx
+++ b/resources/excel_config.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
   <si>
     <t xml:space="preserve">Проект</t>
   </si>
@@ -60,6 +60,21 @@
     <t xml:space="preserve">Значение</t>
   </si>
   <si>
+    <t xml:space="preserve">Комментарий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pupilsPerCitizen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Доля учеников среди жителей</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lackPenaltyCoefficient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Коэффициент для штрафа за нехватку учебных мест</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID ограничения</t>
   </si>
   <si>
@@ -69,31 +84,70 @@
     <t xml:space="preserve">beach</t>
   </si>
   <si>
+    <t xml:space="preserve">пляж</t>
+  </si>
+  <si>
     <t xml:space="preserve">gas-station</t>
   </si>
   <si>
+    <t xml:space="preserve">заправочные станции</t>
+  </si>
+  <si>
     <t xml:space="preserve">industrial-area</t>
   </si>
   <si>
+    <t xml:space="preserve">промзоны</t>
+  </si>
+  <si>
     <t xml:space="preserve">nuklear-zone</t>
   </si>
   <si>
+    <t xml:space="preserve">радиозоны</t>
+  </si>
+  <si>
     <t xml:space="preserve">snow-melting-station</t>
   </si>
   <si>
+    <t xml:space="preserve">зоны плавки снега</t>
+  </si>
+  <si>
     <t xml:space="preserve">transport-nodes</t>
   </si>
   <si>
+    <t xml:space="preserve">транспортные узлы</t>
+  </si>
+  <si>
     <t xml:space="preserve">water</t>
   </si>
   <si>
+    <t xml:space="preserve">вода</t>
+  </si>
+  <si>
     <t xml:space="preserve">highway</t>
   </si>
   <si>
+    <t xml:space="preserve">дороги</t>
+  </si>
+  <si>
     <t xml:space="preserve">park</t>
   </si>
   <si>
+    <t xml:space="preserve">Нет</t>
+  </si>
+  <si>
+    <t xml:space="preserve">парки</t>
+  </si>
+  <si>
     <t xml:space="preserve">building</t>
+  </si>
+  <si>
+    <t xml:space="preserve">здания</t>
+  </si>
+  <si>
+    <t xml:space="preserve">railroad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">железные дороги</t>
   </si>
 </sst>
 </file>
@@ -108,6 +162,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -197,9 +252,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="27.9438775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,18 +355,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.4234693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.9948979591837"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -323,11 +375,36 @@
       <c r="B1" s="0" t="s">
         <v>11</v>
       </c>
+      <c r="C1" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>
@@ -340,33 +417,36 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
+      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4540816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="30.3724489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="C1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>0.1</v>
@@ -374,10 +454,13 @@
       <c r="C2" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="D2" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>0.05</v>
@@ -385,10 +468,13 @@
       <c r="C3" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="D3" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>0.05</v>
@@ -396,10 +482,13 @@
       <c r="C4" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>0.2</v>
@@ -407,10 +496,13 @@
       <c r="C5" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="D5" s="0" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>0.1</v>
@@ -418,10 +510,13 @@
       <c r="C6" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="D6" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>0.1</v>
@@ -429,10 +524,13 @@
       <c r="C7" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="D7" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.1</v>
@@ -440,10 +538,13 @@
       <c r="C8" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="D8" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0.05</v>
@@ -451,33 +552,56 @@
       <c r="C9" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="D9" s="0" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>0.001</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>5</v>
+        <v>36</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>0.05</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>5</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Обычный"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Обычный"&amp;12Страница &amp;P</oddFooter>

</xml_diff>